<commit_message>
PP, both options full and selected should be working now
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>product_code</t>
   </si>
@@ -43,16 +43,55 @@
   </si>
   <si>
     <t>currency_code</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>asdasdasdsa</t>
+  </si>
+  <si>
+    <t>hsfghfgh</t>
+  </si>
+  <si>
+    <t>CM1008RWD-KALORIK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,13 +114,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -384,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,10 +450,10 @@
     <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,6 +463,9 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
@@ -428,8 +481,33 @@
       <c r="I1" t="s">
         <v>1</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
     </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
PP, photo attachment should be workking now
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>product_code</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>CM1008RWD-KALORIK</t>
+  </si>
+  <si>
+    <t>file_name</t>
+  </si>
+  <si>
+    <t>tile_file_name</t>
   </si>
 </sst>
 </file>
@@ -434,26 +440,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,28 +493,34 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
PP, photos now working for selected
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>product_code</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>tile_file_name</t>
+  </si>
+  <si>
+    <t>BSET1000-KALORIK</t>
+  </si>
+  <si>
+    <t>photo</t>
   </si>
 </sst>
 </file>
@@ -440,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +468,7 @@
     <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,28 +505,36 @@
       <c r="L1" t="s">
         <v>14</v>
       </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
PP, generate all should be working as well
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>product_code</t>
   </si>
@@ -51,22 +51,10 @@
     <t>range</t>
   </si>
   <si>
-    <t>asdasdasdsa</t>
-  </si>
-  <si>
-    <t>hsfghfgh</t>
-  </si>
-  <si>
-    <t>CM1008RWD-KALORIK</t>
-  </si>
-  <si>
     <t>file_name</t>
   </si>
   <si>
     <t>tile_file_name</t>
-  </si>
-  <si>
-    <t>BSET1000-KALORIK</t>
   </si>
   <si>
     <t>photo</t>
@@ -93,9 +81,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="24"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,6 +94,7 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -128,18 +117,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -446,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +455,7 @@
     <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,41 +487,855 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="7" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+    </row>
+    <row r="12" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+    </row>
+    <row r="13" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
PP, selected almost working on async
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="1083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="1084">
   <si>
     <t>product_code</t>
   </si>
@@ -3269,6 +3269,9 @@
   </si>
   <si>
     <t>ZWE1000-SCHOTT</t>
+  </si>
+  <si>
+    <t>Z3 ZESTAW</t>
   </si>
 </sst>
 </file>
@@ -3624,7 +3627,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3694,6 +3697,16 @@
         <v>78</v>
       </c>
     </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1083</v>
+      </c>
+    </row>
     <row r="12" spans="1:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>

<commit_message>
PP, comit test scripts
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="1084">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="1083">
   <si>
     <t>product_code</t>
   </si>
@@ -3269,9 +3269,6 @@
   </si>
   <si>
     <t>ZWE1000-SCHOTT</t>
-  </si>
-  <si>
-    <t>Z3 ZESTAW</t>
   </si>
 </sst>
 </file>
@@ -3627,7 +3624,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3688,23 +3685,14 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1083</v>
+      <c r="A3" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
PP, should be stable now
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="1083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="1085">
   <si>
     <t>product_code</t>
   </si>
@@ -3269,6 +3269,12 @@
   </si>
   <si>
     <t>ZWE1000-SCHOTT</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
   </si>
 </sst>
 </file>
@@ -3621,15 +3627,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
@@ -3641,6 +3647,7 @@
     <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -3688,15 +3695,225 @@
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1084</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
PP, selected should be working
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORK\team\team.reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2669C1DA-B43A-44C0-81BD-BD5810AD2412}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B078D18F-EEE8-4B74-BDA0-43C2E3D2D0D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="1109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="1112">
   <si>
     <t>product_code</t>
   </si>
@@ -3348,6 +3348,15 @@
   </si>
   <si>
     <t>tile_url</t>
+  </si>
+  <si>
+    <t>features</t>
+  </si>
+  <si>
+    <t>features_trans</t>
+  </si>
+  <si>
+    <t>locale_code</t>
   </si>
 </sst>
 </file>
@@ -3436,7 +3445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3451,6 +3460,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -3789,55 +3804,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK33"/>
+  <dimension ref="A1:AN33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5546875" style="9" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="3.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="3.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="8.88671875" style="5"/>
+    <col min="3" max="3" width="7.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3845,246 +3863,351 @@
         <v>1106</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1110</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1111</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>1081</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>1082</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>1083</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>1084</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>1085</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>1086</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>1087</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>1088</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>1089</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>1090</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>1091</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>1092</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>1093</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>1094</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>1095</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>1096</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>1097</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>1098</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>1099</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>1101</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>1102</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>1103</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>1104</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>1105</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>1108</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>180</v>
       </c>
       <c r="B2" s="6"/>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>181</v>
       </c>
       <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>182</v>
       </c>
       <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>1107</v>
       </c>
       <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>